<commit_message>
add: promps & sells
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -47,10 +47,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF98BB6C"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <sz val="8"/>
+      <color rgb="FF121214"/>
+      <name val="Roboto"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -74,12 +73,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -384,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,9 +406,105 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>